<commit_message>
Updated Test Data and imports
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\321020\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347FD2BC-67B7-4EC5-83C3-F47794324737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDD5605-2628-47A4-964E-25184A571723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProject" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>UserID</t>
   </si>
   <si>
-    <t>data1</t>
-  </si>
-  <si>
     <t>data2</t>
   </si>
   <si>
@@ -85,10 +82,13 @@
     <t>data3</t>
   </si>
   <si>
+    <t>TD004</t>
+  </si>
+  <si>
+    <t>data5</t>
+  </si>
+  <si>
     <t>Lot 2</t>
-  </si>
-  <si>
-    <t>TD004</t>
   </si>
 </sst>
 </file>
@@ -448,9 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F461487-BD88-45EF-A8A5-6601D1401C9D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -476,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -490,7 +488,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -501,10 +499,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -515,16 +513,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CA7865-3918-4BA1-BE24-25DC7217DA00}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added code for RFI journey
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\321020\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347FD2BC-67B7-4EC5-83C3-F47794324737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA1C3DB-9F52-4ADF-A793-98ED08386395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProject" sheetId="1" r:id="rId1"/>
     <sheet name="UpdateProject" sheetId="2" r:id="rId2"/>
+    <sheet name="OneFCFlowTestData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>TDID</t>
   </si>
@@ -89,6 +90,70 @@
   </si>
   <si>
     <t>TD004</t>
+  </si>
+  <si>
+    <t>Dashboard_PageTitle</t>
+  </si>
+  <si>
+    <t>ChooseAgreemnt_PageTitle</t>
+  </si>
+  <si>
+    <t>ProcOverview_PageTitle</t>
+  </si>
+  <si>
+    <t>Find suppliers and run your procurement online.</t>
+  </si>
+  <si>
+    <t>Choose a commercial agreement</t>
+  </si>
+  <si>
+    <t>Lot 1: Digital Programmes</t>
+  </si>
+  <si>
+    <t>Procurement overview</t>
+  </si>
+  <si>
+    <t>Lot 2: Digital Specialists</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>feedback (opens in a new window)</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>SelectedAgreement</t>
+  </si>
+  <si>
+    <t>HelpSection</t>
+  </si>
+  <si>
+    <t>Digital Specialists and Programmes, Lot 1: Digital Programmes!RM6263!RM6263-Lot 1-COGNIZANT BUSINESS SERVICES UK LIMITED</t>
+  </si>
+  <si>
+    <t>enquiry form
+Opens in a new tab!0345 410 2222!info@crowncommercial.gov.uk!CCS customer services team is available Monday to Friday, 9am to 5pm.</t>
+  </si>
+  <si>
+    <t>contact us!Terms and conditions!Privacy policy!Cookie policy!Accessibility statement!© Crown copyright</t>
+  </si>
+  <si>
+    <t>ProcurementOverviewPageContentButtonStatus</t>
+  </si>
+  <si>
+    <t>My account!Sign out!Contract Award Service!Home!My Projects!CCS website!Guidance!Get help</t>
+  </si>
+  <si>
+    <t>1. See available suppliers!OPTIONAL!See available suppliers!2. Do pre-market engagement!OPTIONAL!Start pre-market engagement!3. Write and publish your requirements!TODO!Write and publish your requirements!4. Do evaluation!CANNOT START YET!5. Award the contract!CANNOT START YET!6. Publish your contract!OPTIONAL</t>
   </si>
 </sst>
 </file>
@@ -130,8 +195,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,12 +523,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -485,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -499,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -513,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -538,18 +609,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CA7865-3918-4BA1-BE24-25DC7217DA00}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -571,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -586,4 +657,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA8D49A-BB20-4C74-9F3C-A1F46BC5FE7B}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="41.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>